<commit_message>
Simulation 1: multiple conditions of sample size split
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC960CAF-8D5C-4C8A-AE78-F4961417D515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4E401-3638-4EB9-B204-ECF4BEF82005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,37 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
-  <si>
-    <t>Study 1</t>
-  </si>
-  <si>
-    <t>Study 2</t>
-  </si>
-  <si>
-    <t>Study 3</t>
-  </si>
-  <si>
-    <t>Study 4</t>
-  </si>
-  <si>
-    <t>Study 5</t>
-  </si>
-  <si>
-    <t>Study 6</t>
-  </si>
-  <si>
-    <t>Study 7</t>
-  </si>
-  <si>
-    <t>Study 8</t>
-  </si>
-  <si>
-    <t>Study 9</t>
-  </si>
-  <si>
-    <t>Study 10</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Condition</t>
   </si>
@@ -119,6 +89,48 @@
   </si>
   <si>
     <t xml:space="preserve">2-2-2-2-1-1 continuous </t>
+  </si>
+  <si>
+    <t>Condition.wording</t>
+  </si>
+  <si>
+    <t>Study.1</t>
+  </si>
+  <si>
+    <t>Study.2</t>
+  </si>
+  <si>
+    <t>Study.3</t>
+  </si>
+  <si>
+    <t>Study.4</t>
+  </si>
+  <si>
+    <t>Study.5</t>
+  </si>
+  <si>
+    <t>Study.6</t>
+  </si>
+  <si>
+    <t>Study.7</t>
+  </si>
+  <si>
+    <t>Study.8</t>
+  </si>
+  <si>
+    <t>Study.9</t>
+  </si>
+  <si>
+    <t>Study.10</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>control condition</t>
+  </si>
+  <si>
+    <t>can few very well powered studies compensate for the rest of underpowered studies?</t>
   </si>
 </sst>
 </file>
@@ -261,9 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -308,6 +317,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,398 +609,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.109375" customWidth="1"/>
     <col min="2" max="2" width="46.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="8.88671875" style="4"/>
-    <col min="12" max="12" width="8.88671875" style="4"/>
-    <col min="13" max="13" width="24.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="12" max="12" width="8.88671875" style="3"/>
+    <col min="13" max="13" width="24.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="27" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B1" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>9</v>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21">
+        <v>200</v>
+      </c>
+      <c r="D2" s="22">
+        <v>200</v>
+      </c>
+      <c r="E2" s="22">
+        <v>200</v>
+      </c>
+      <c r="F2" s="22">
+        <v>200</v>
+      </c>
+      <c r="G2" s="22">
+        <v>200</v>
+      </c>
+      <c r="H2" s="21">
+        <v>200</v>
+      </c>
+      <c r="I2" s="22">
+        <v>200</v>
+      </c>
+      <c r="J2" s="22">
+        <v>200</v>
+      </c>
+      <c r="K2" s="22">
+        <v>200</v>
+      </c>
+      <c r="L2" s="21">
+        <v>200</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="20">
+        <v>100</v>
+      </c>
+      <c r="D3" s="20">
+        <v>100</v>
+      </c>
+      <c r="E3" s="20">
+        <v>100</v>
+      </c>
+      <c r="F3" s="20">
+        <v>100</v>
+      </c>
+      <c r="G3" s="20">
+        <v>100</v>
+      </c>
+      <c r="H3" s="23">
+        <v>300</v>
+      </c>
+      <c r="I3" s="23">
+        <v>300</v>
+      </c>
+      <c r="J3" s="24">
+        <v>300</v>
+      </c>
+      <c r="K3" s="24">
+        <v>300</v>
+      </c>
+      <c r="L3" s="23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="22">
-        <v>200</v>
-      </c>
-      <c r="D3" s="23">
-        <v>200</v>
-      </c>
-      <c r="E3" s="23">
-        <v>200</v>
-      </c>
-      <c r="F3" s="23">
-        <v>200</v>
-      </c>
-      <c r="G3" s="23">
-        <v>200</v>
-      </c>
-      <c r="H3" s="22">
-        <v>200</v>
-      </c>
-      <c r="I3" s="23">
-        <v>200</v>
-      </c>
-      <c r="J3" s="23">
-        <v>200</v>
-      </c>
-      <c r="K3" s="23">
-        <v>200</v>
-      </c>
-      <c r="L3" s="22">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1.2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="21">
-        <v>100</v>
-      </c>
-      <c r="D4" s="21">
-        <v>100</v>
-      </c>
-      <c r="E4" s="21">
-        <v>100</v>
-      </c>
-      <c r="F4" s="21">
-        <v>100</v>
-      </c>
-      <c r="G4" s="21">
-        <v>100</v>
-      </c>
-      <c r="H4" s="24">
-        <v>300</v>
+      <c r="C4" s="9">
+        <v>50</v>
+      </c>
+      <c r="D4" s="8">
+        <v>50</v>
+      </c>
+      <c r="E4" s="8">
+        <v>50</v>
+      </c>
+      <c r="F4" s="8">
+        <v>50</v>
+      </c>
+      <c r="G4" s="8">
+        <v>50</v>
+      </c>
+      <c r="H4" s="23">
+        <v>350</v>
       </c>
       <c r="I4" s="24">
-        <v>300</v>
-      </c>
-      <c r="J4" s="25">
-        <v>300</v>
-      </c>
-      <c r="K4" s="25">
-        <v>300</v>
-      </c>
-      <c r="L4" s="24">
-        <v>300</v>
+        <v>350</v>
+      </c>
+      <c r="J4" s="24">
+        <v>350</v>
+      </c>
+      <c r="K4" s="24">
+        <v>350</v>
+      </c>
+      <c r="L4" s="23">
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1.3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="10">
-        <v>50</v>
-      </c>
-      <c r="D5" s="9">
-        <v>50</v>
-      </c>
-      <c r="E5" s="9">
-        <v>50</v>
-      </c>
-      <c r="F5" s="9">
-        <v>50</v>
-      </c>
-      <c r="G5" s="9">
-        <v>50</v>
-      </c>
-      <c r="H5" s="24">
-        <v>350</v>
-      </c>
-      <c r="I5" s="25">
-        <v>350</v>
-      </c>
-      <c r="J5" s="25">
-        <v>350</v>
-      </c>
-      <c r="K5" s="25">
-        <v>350</v>
-      </c>
-      <c r="L5" s="24">
-        <v>350</v>
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19">
+        <v>25</v>
+      </c>
+      <c r="E5" s="19">
+        <v>25</v>
+      </c>
+      <c r="F5" s="21">
+        <v>200</v>
+      </c>
+      <c r="G5" s="21">
+        <v>200</v>
+      </c>
+      <c r="H5" s="21">
+        <v>200</v>
+      </c>
+      <c r="I5" s="22">
+        <v>200</v>
+      </c>
+      <c r="J5" s="24">
+        <v>375</v>
+      </c>
+      <c r="K5" s="24">
+        <v>375</v>
+      </c>
+      <c r="L5" s="23">
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>25</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>25</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <v>25</v>
       </c>
-      <c r="F6" s="22">
-        <v>200</v>
-      </c>
-      <c r="G6" s="22">
-        <v>200</v>
-      </c>
-      <c r="H6" s="22">
-        <v>200</v>
-      </c>
-      <c r="I6" s="23">
-        <v>200</v>
+      <c r="F6" s="9">
+        <v>50</v>
+      </c>
+      <c r="G6" s="9">
+        <v>50</v>
+      </c>
+      <c r="H6" s="9">
+        <v>50</v>
+      </c>
+      <c r="I6" s="8">
+        <v>50</v>
       </c>
       <c r="J6" s="25">
-        <v>375</v>
+        <v>575</v>
       </c>
       <c r="K6" s="25">
-        <v>375</v>
-      </c>
-      <c r="L6" s="24">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>575</v>
+      </c>
+      <c r="L6" s="28">
+        <v>575</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="20">
+        <v>19</v>
+      </c>
+      <c r="C7" s="19">
         <v>25</v>
       </c>
       <c r="D7" s="20">
+        <v>100</v>
+      </c>
+      <c r="E7" s="20">
+        <v>100</v>
+      </c>
+      <c r="F7" s="20">
+        <v>100</v>
+      </c>
+      <c r="G7" s="20">
+        <v>100</v>
+      </c>
+      <c r="H7" s="21">
+        <v>200</v>
+      </c>
+      <c r="I7" s="21">
+        <v>200</v>
+      </c>
+      <c r="J7" s="21">
+        <v>200</v>
+      </c>
+      <c r="K7" s="21">
+        <v>200</v>
+      </c>
+      <c r="L7" s="29">
+        <v>775</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19">
         <v>25</v>
       </c>
-      <c r="E7" s="20">
+      <c r="D8" s="9">
+        <v>50</v>
+      </c>
+      <c r="E8" s="9">
+        <v>50</v>
+      </c>
+      <c r="F8" s="9">
+        <v>50</v>
+      </c>
+      <c r="G8" s="9">
+        <v>50</v>
+      </c>
+      <c r="H8" s="20">
+        <v>100</v>
+      </c>
+      <c r="I8" s="20">
+        <v>100</v>
+      </c>
+      <c r="J8" s="20">
+        <v>100</v>
+      </c>
+      <c r="K8" s="20">
+        <v>100</v>
+      </c>
+      <c r="L8" s="10">
+        <v>1375</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9">
+        <v>50</v>
+      </c>
+      <c r="D9" s="9">
+        <v>50</v>
+      </c>
+      <c r="E9" s="9">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9">
+        <v>50</v>
+      </c>
+      <c r="G9" s="9">
+        <v>50</v>
+      </c>
+      <c r="H9" s="9">
+        <v>50</v>
+      </c>
+      <c r="I9" s="9">
+        <v>50</v>
+      </c>
+      <c r="J9" s="9">
+        <v>50</v>
+      </c>
+      <c r="K9" s="9">
+        <v>50</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1550</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19">
         <v>25</v>
       </c>
-      <c r="F7" s="10">
-        <v>50</v>
-      </c>
-      <c r="G7" s="10">
-        <v>50</v>
-      </c>
-      <c r="H7" s="10">
-        <v>50</v>
-      </c>
-      <c r="I7" s="9">
-        <v>50</v>
-      </c>
-      <c r="J7" s="26">
-        <v>575</v>
-      </c>
-      <c r="K7" s="26">
-        <v>575</v>
-      </c>
-      <c r="L7" s="29">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="20">
+      <c r="D10" s="19">
         <v>25</v>
       </c>
-      <c r="D8" s="21">
-        <v>100</v>
-      </c>
-      <c r="E8" s="21">
-        <v>100</v>
-      </c>
-      <c r="F8" s="21">
-        <v>100</v>
-      </c>
-      <c r="G8" s="21">
-        <v>100</v>
-      </c>
-      <c r="H8" s="22">
-        <v>200</v>
-      </c>
-      <c r="I8" s="22">
-        <v>200</v>
-      </c>
-      <c r="J8" s="22">
-        <v>200</v>
-      </c>
-      <c r="K8" s="22">
-        <v>200</v>
-      </c>
-      <c r="L8" s="30">
-        <v>780</v>
-      </c>
-      <c r="M8" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="20">
-        <v>25</v>
-      </c>
-      <c r="D9" s="10">
-        <v>50</v>
-      </c>
-      <c r="E9" s="10">
-        <v>50</v>
-      </c>
-      <c r="F9" s="10">
-        <v>50</v>
-      </c>
-      <c r="G9" s="10">
-        <v>50</v>
-      </c>
-      <c r="H9" s="21">
-        <v>100</v>
-      </c>
-      <c r="I9" s="21">
-        <v>100</v>
-      </c>
-      <c r="J9" s="21">
-        <v>100</v>
-      </c>
-      <c r="K9" s="21">
-        <v>100</v>
-      </c>
-      <c r="L9" s="11">
-        <v>1375</v>
-      </c>
-      <c r="M9" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="10">
-        <v>50</v>
-      </c>
-      <c r="D10" s="10">
-        <v>50</v>
-      </c>
-      <c r="E10" s="10">
-        <v>50</v>
-      </c>
-      <c r="F10" s="10">
-        <v>50</v>
-      </c>
-      <c r="G10" s="10">
-        <v>50</v>
-      </c>
-      <c r="H10" s="10">
-        <v>50</v>
-      </c>
-      <c r="I10" s="10">
-        <v>50</v>
-      </c>
-      <c r="J10" s="10">
-        <v>50</v>
-      </c>
-      <c r="K10" s="10">
-        <v>50</v>
-      </c>
-      <c r="L10" s="11">
-        <v>1550</v>
-      </c>
-      <c r="M10" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="20">
-        <v>25</v>
-      </c>
-      <c r="D11" s="20">
-        <v>25</v>
-      </c>
-      <c r="E11" s="10">
-        <v>50</v>
-      </c>
-      <c r="F11" s="10">
-        <v>50</v>
-      </c>
-      <c r="G11" s="21">
-        <v>100</v>
-      </c>
-      <c r="H11" s="21">
-        <v>100</v>
-      </c>
-      <c r="I11" s="22">
-        <v>200</v>
-      </c>
-      <c r="J11" s="22">
-        <v>200</v>
-      </c>
-      <c r="K11" s="25">
+      <c r="E10" s="9">
+        <v>50</v>
+      </c>
+      <c r="F10" s="9">
+        <v>50</v>
+      </c>
+      <c r="G10" s="20">
+        <v>100</v>
+      </c>
+      <c r="H10" s="20">
+        <v>100</v>
+      </c>
+      <c r="I10" s="21">
+        <v>200</v>
+      </c>
+      <c r="J10" s="21">
+        <v>200</v>
+      </c>
+      <c r="K10" s="24">
         <v>400</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L10" s="29">
         <v>850</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1011,96 +1046,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="A2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="3">
+        <v>200</v>
+      </c>
+      <c r="E3" s="4">
+        <v>300</v>
+      </c>
+      <c r="F3" s="3">
+        <v>400</v>
+      </c>
+      <c r="G3" s="4">
+        <v>500</v>
+      </c>
+      <c r="H3" s="4">
+        <v>600</v>
+      </c>
+      <c r="I3" s="4">
+        <v>700</v>
+      </c>
+      <c r="J3" s="3">
+        <v>800</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4">
-        <v>50</v>
-      </c>
-      <c r="C3" s="4">
-        <v>100</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="5">
-        <v>300</v>
-      </c>
-      <c r="F3" s="4">
-        <v>400</v>
-      </c>
-      <c r="G3" s="5">
-        <v>500</v>
-      </c>
-      <c r="H3" s="5">
-        <v>600</v>
-      </c>
-      <c r="I3" s="5">
-        <v>700</v>
-      </c>
-      <c r="J3" s="4">
-        <v>800</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Simulation 1 (10 studies): Results
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,25 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4E401-3638-4EB9-B204-ECF4BEF82005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4398AD-9565-47B2-BB1D-46477115B0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sim1 N=4000" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Condition</t>
   </si>
@@ -611,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1031,6 +1043,428 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9070EDF0-829D-4F07-965D-C082A11BFB0B}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="46.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="12" max="12" width="8.88671875" style="3"/>
+    <col min="13" max="13" width="24.6640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21">
+        <v>100</v>
+      </c>
+      <c r="D2" s="21">
+        <v>100</v>
+      </c>
+      <c r="E2" s="21">
+        <v>100</v>
+      </c>
+      <c r="F2" s="21">
+        <v>100</v>
+      </c>
+      <c r="G2" s="21">
+        <v>100</v>
+      </c>
+      <c r="H2" s="21">
+        <v>100</v>
+      </c>
+      <c r="I2" s="21">
+        <v>100</v>
+      </c>
+      <c r="J2" s="21">
+        <v>100</v>
+      </c>
+      <c r="K2" s="21">
+        <v>100</v>
+      </c>
+      <c r="L2" s="21">
+        <v>100</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="20">
+        <v>50</v>
+      </c>
+      <c r="D3" s="20">
+        <v>50</v>
+      </c>
+      <c r="E3" s="20">
+        <v>50</v>
+      </c>
+      <c r="F3" s="20">
+        <v>50</v>
+      </c>
+      <c r="G3" s="20">
+        <v>50</v>
+      </c>
+      <c r="H3" s="23">
+        <v>150</v>
+      </c>
+      <c r="I3" s="23">
+        <v>150</v>
+      </c>
+      <c r="J3" s="23">
+        <v>150</v>
+      </c>
+      <c r="K3" s="23">
+        <v>150</v>
+      </c>
+      <c r="L3" s="23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9">
+        <v>25</v>
+      </c>
+      <c r="E4" s="9">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9">
+        <v>25</v>
+      </c>
+      <c r="G4" s="9">
+        <v>25</v>
+      </c>
+      <c r="H4" s="23">
+        <v>175</v>
+      </c>
+      <c r="I4" s="23">
+        <v>175</v>
+      </c>
+      <c r="J4" s="23">
+        <v>175</v>
+      </c>
+      <c r="K4" s="23">
+        <v>175</v>
+      </c>
+      <c r="L4" s="23">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19">
+        <v>25</v>
+      </c>
+      <c r="E5" s="19">
+        <v>25</v>
+      </c>
+      <c r="F5" s="21">
+        <v>100</v>
+      </c>
+      <c r="G5" s="21">
+        <v>100</v>
+      </c>
+      <c r="H5" s="21">
+        <v>100</v>
+      </c>
+      <c r="I5" s="21">
+        <v>100</v>
+      </c>
+      <c r="J5" s="24">
+        <v>175</v>
+      </c>
+      <c r="K5" s="24">
+        <v>175</v>
+      </c>
+      <c r="L5" s="24">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="19">
+        <v>25</v>
+      </c>
+      <c r="D6" s="19">
+        <v>25</v>
+      </c>
+      <c r="E6" s="19">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9">
+        <v>45</v>
+      </c>
+      <c r="G6" s="9">
+        <v>45</v>
+      </c>
+      <c r="H6" s="9">
+        <v>45</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45</v>
+      </c>
+      <c r="J6" s="25">
+        <v>245</v>
+      </c>
+      <c r="K6" s="25">
+        <v>250</v>
+      </c>
+      <c r="L6" s="25">
+        <v>250</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="19">
+        <v>25</v>
+      </c>
+      <c r="D7" s="20">
+        <v>50</v>
+      </c>
+      <c r="E7" s="20">
+        <v>50</v>
+      </c>
+      <c r="F7" s="20">
+        <v>50</v>
+      </c>
+      <c r="G7" s="20">
+        <v>50</v>
+      </c>
+      <c r="H7" s="21">
+        <v>100</v>
+      </c>
+      <c r="I7" s="21">
+        <v>100</v>
+      </c>
+      <c r="J7" s="21">
+        <v>100</v>
+      </c>
+      <c r="K7" s="21">
+        <v>100</v>
+      </c>
+      <c r="L7" s="29">
+        <v>375</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19">
+        <v>25</v>
+      </c>
+      <c r="D8" s="9">
+        <v>50</v>
+      </c>
+      <c r="E8" s="9">
+        <v>50</v>
+      </c>
+      <c r="F8" s="9">
+        <v>50</v>
+      </c>
+      <c r="G8" s="9">
+        <v>50</v>
+      </c>
+      <c r="H8" s="20">
+        <v>100</v>
+      </c>
+      <c r="I8" s="20">
+        <v>100</v>
+      </c>
+      <c r="J8" s="20">
+        <v>100</v>
+      </c>
+      <c r="K8" s="20">
+        <v>100</v>
+      </c>
+      <c r="L8" s="29">
+        <v>375</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9">
+        <v>25</v>
+      </c>
+      <c r="D9" s="9">
+        <v>25</v>
+      </c>
+      <c r="E9" s="9">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9">
+        <v>25</v>
+      </c>
+      <c r="H9" s="9">
+        <v>25</v>
+      </c>
+      <c r="I9" s="9">
+        <v>25</v>
+      </c>
+      <c r="J9" s="9">
+        <v>25</v>
+      </c>
+      <c r="K9" s="9">
+        <v>25</v>
+      </c>
+      <c r="L9" s="10">
+        <v>775</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19">
+        <v>25</v>
+      </c>
+      <c r="D10" s="19">
+        <v>25</v>
+      </c>
+      <c r="E10" s="19">
+        <v>25</v>
+      </c>
+      <c r="F10" s="19">
+        <v>25</v>
+      </c>
+      <c r="G10" s="20">
+        <v>50</v>
+      </c>
+      <c r="H10" s="20">
+        <v>50</v>
+      </c>
+      <c r="I10" s="21">
+        <v>100</v>
+      </c>
+      <c r="J10" s="21">
+        <v>100</v>
+      </c>
+      <c r="K10" s="24">
+        <v>200</v>
+      </c>
+      <c r="L10" s="29">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C1D6A-9ED8-4638-8561-F699B52D61B5}">
   <dimension ref="A1:K5"/>
   <sheetViews>

</xml_diff>

<commit_message>
update plot Sim 1
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065D06DA-F7A2-434C-8DDE-5C7056653250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C9051E-2EEE-4BEE-8A8C-426B2F6A1B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="4" r:id="rId1"/>
     <sheet name="Sim1_Ntotal=2000" sheetId="1" r:id="rId2"/>
     <sheet name="Sim1_Ntotal=1000" sheetId="3" r:id="rId3"/>
     <sheet name="Degrees of power" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Power quantification" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Condition</t>
   </si>
@@ -172,13 +173,263 @@
   </si>
   <si>
     <t>can multiple somewhat underpowered studies (p=0.7) accumulate evidence for the true hypothesis</t>
+  </si>
+  <si>
+    <t>0.5/0.55</t>
+  </si>
+  <si>
+    <t>condition    correct.aggr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF949494"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;chr&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">               </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF949494"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;dbl&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.1         0.605</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.2         0.734</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.3         0.862</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.4         0.932</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.5         0.972</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.6         0.994</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.7         0.998</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.8         1    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.9         1    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.10        1   </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.1        0.600</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.2        0.740</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.3        0.933</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.4        0.994</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Condition.5        1   </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +451,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF949494"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFBCBCBC"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +523,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEF8C4F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,13 +643,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E3F23-FB2A-4BE0-9E04-457B31D94BA1}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,41 +998,41 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="30" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" s="33">
+      <c r="H2">
         <v>10</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2">
         <v>10</v>
       </c>
-      <c r="L2" s="33">
+      <c r="L2">
         <v>10</v>
       </c>
     </row>
@@ -801,40 +1082,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="C4" s="31">
-        <v>104</v>
-      </c>
-      <c r="D4" s="31">
-        <v>104</v>
-      </c>
-      <c r="E4" s="31">
-        <v>104</v>
-      </c>
-      <c r="F4" s="31">
-        <v>104</v>
-      </c>
-      <c r="G4" s="31">
-        <v>104</v>
-      </c>
-      <c r="H4" s="31">
-        <v>104</v>
-      </c>
-      <c r="I4" s="31">
-        <v>104</v>
-      </c>
-      <c r="J4" s="31">
-        <v>104</v>
-      </c>
-      <c r="K4" s="31">
-        <v>104</v>
-      </c>
-      <c r="L4" s="31">
-        <v>104</v>
-      </c>
-      <c r="M4" t="s">
-        <v>43</v>
+        <v>0.65</v>
+      </c>
+      <c r="C4">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>55</v>
+      </c>
+      <c r="G4">
+        <v>55</v>
+      </c>
+      <c r="H4">
+        <v>55</v>
+      </c>
+      <c r="I4">
+        <v>55</v>
+      </c>
+      <c r="J4">
+        <v>55</v>
+      </c>
+      <c r="K4">
+        <v>55</v>
+      </c>
+      <c r="L4">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -842,37 +1120,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="32">
-        <v>257</v>
-      </c>
-      <c r="D5" s="32">
-        <v>257</v>
-      </c>
-      <c r="E5" s="32">
-        <v>257</v>
-      </c>
-      <c r="F5" s="32">
-        <v>257</v>
-      </c>
-      <c r="G5" s="32">
-        <v>257</v>
-      </c>
-      <c r="H5" s="32">
-        <v>257</v>
-      </c>
-      <c r="I5" s="32">
-        <v>257</v>
-      </c>
-      <c r="J5" s="32">
-        <v>257</v>
-      </c>
-      <c r="K5" s="32">
-        <v>257</v>
-      </c>
-      <c r="L5" s="32">
-        <v>257</v>
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>104</v>
+      </c>
+      <c r="D5">
+        <v>104</v>
+      </c>
+      <c r="E5">
+        <v>104</v>
+      </c>
+      <c r="F5">
+        <v>104</v>
+      </c>
+      <c r="G5">
+        <v>104</v>
+      </c>
+      <c r="H5">
+        <v>104</v>
+      </c>
+      <c r="I5">
+        <v>104</v>
+      </c>
+      <c r="J5">
+        <v>104</v>
+      </c>
+      <c r="K5">
+        <v>104</v>
+      </c>
+      <c r="L5">
+        <v>104</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -880,92 +1161,235 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C6">
+        <v>167</v>
+      </c>
+      <c r="D6">
+        <v>167</v>
+      </c>
+      <c r="E6">
+        <v>167</v>
+      </c>
+      <c r="F6">
+        <v>167</v>
+      </c>
+      <c r="G6">
+        <v>167</v>
+      </c>
+      <c r="H6">
+        <v>167</v>
+      </c>
+      <c r="I6">
+        <v>167</v>
+      </c>
+      <c r="J6">
+        <v>167</v>
+      </c>
+      <c r="K6">
+        <v>167</v>
+      </c>
+      <c r="L6">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="29">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C7">
+        <v>257</v>
+      </c>
+      <c r="D7">
+        <v>257</v>
+      </c>
+      <c r="E7">
+        <v>257</v>
+      </c>
+      <c r="F7">
+        <v>257</v>
+      </c>
+      <c r="G7">
+        <v>257</v>
+      </c>
+      <c r="H7">
+        <v>257</v>
+      </c>
+      <c r="I7">
+        <v>257</v>
+      </c>
+      <c r="J7">
+        <v>257</v>
+      </c>
+      <c r="K7">
+        <v>257</v>
+      </c>
+      <c r="L7">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C8">
+        <v>391</v>
+      </c>
+      <c r="D8">
+        <v>391</v>
+      </c>
+      <c r="E8">
+        <v>391</v>
+      </c>
+      <c r="F8">
+        <v>391</v>
+      </c>
+      <c r="G8">
+        <v>391</v>
+      </c>
+      <c r="H8">
+        <v>391</v>
+      </c>
+      <c r="I8">
+        <v>391</v>
+      </c>
+      <c r="J8">
+        <v>391</v>
+      </c>
+      <c r="K8">
+        <v>391</v>
+      </c>
+      <c r="L8">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>0.9</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>586</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <v>586</v>
       </c>
-      <c r="E6">
+      <c r="E9">
         <v>586</v>
       </c>
-      <c r="F6">
+      <c r="F9">
         <v>586</v>
       </c>
-      <c r="G6">
+      <c r="G9">
         <v>586</v>
       </c>
-      <c r="H6">
+      <c r="H9">
         <v>586</v>
       </c>
-      <c r="I6">
+      <c r="I9">
         <v>586</v>
       </c>
-      <c r="J6">
+      <c r="J9">
         <v>586</v>
       </c>
-      <c r="K6">
+      <c r="K9">
         <v>586</v>
       </c>
-      <c r="L6">
+      <c r="L9">
         <v>586</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-    </row>
-    <row r="8" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="19"/>
-    </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
+      <c r="A10" s="29">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="C10">
+        <v>976</v>
+      </c>
+      <c r="D10">
+        <v>976</v>
+      </c>
+      <c r="E10">
+        <v>976</v>
+      </c>
+      <c r="F10">
+        <v>976</v>
+      </c>
+      <c r="G10">
+        <v>976</v>
+      </c>
+      <c r="H10">
+        <v>976</v>
+      </c>
+      <c r="I10">
+        <v>976</v>
+      </c>
+      <c r="J10">
+        <v>976</v>
+      </c>
+      <c r="K10">
+        <v>976</v>
+      </c>
+      <c r="L10">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C11">
+        <v>1952</v>
+      </c>
+      <c r="D11">
+        <v>1952</v>
+      </c>
+      <c r="E11">
+        <v>1952</v>
+      </c>
+      <c r="F11">
+        <v>1952</v>
+      </c>
+      <c r="G11">
+        <v>1952</v>
+      </c>
+      <c r="H11">
+        <v>1952</v>
+      </c>
+      <c r="I11">
+        <v>1952</v>
+      </c>
+      <c r="J11">
+        <v>1952</v>
+      </c>
+      <c r="K11">
+        <v>1952</v>
+      </c>
+      <c r="L11">
+        <v>1952</v>
+      </c>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M13" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1815,16 +2239,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C1D6A-9ED8-4638-8561-F699B52D61B5}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="14.21875" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="1" max="11" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1835,7 +2259,10 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1908,19 +2335,22 @@
       <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="I13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1932,18 +2362,27 @@
         <v>27</v>
       </c>
       <c r="C14">
+        <v>55</v>
+      </c>
+      <c r="D14">
         <v>104</v>
       </c>
-      <c r="D14">
+      <c r="E14">
+        <v>167</v>
+      </c>
+      <c r="F14">
         <v>257</v>
       </c>
-      <c r="E14">
+      <c r="G14">
+        <v>391</v>
+      </c>
+      <c r="H14">
         <v>586</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>976</v>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>1952</v>
       </c>
     </row>
@@ -1955,72 +2394,77 @@
         <v>0.6</v>
       </c>
       <c r="C15">
+        <v>0.65</v>
+      </c>
+      <c r="D15">
         <v>0.7</v>
       </c>
-      <c r="D15">
+      <c r="E15">
+        <v>0.75</v>
+      </c>
+      <c r="F15">
         <v>0.8</v>
       </c>
-      <c r="E15">
+      <c r="G15">
+        <v>0.85</v>
+      </c>
+      <c r="H15">
         <v>0.9</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <v>0.95</v>
       </c>
-      <c r="G15">
+      <c r="J15">
         <v>0.99</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I19">
+    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L19">
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I20">
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L20">
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I21">
+    <row r="21" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L21">
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I22">
+    <row r="22" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L22">
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I23">
+    <row r="23" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L23">
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I24">
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L24">
         <v>0.95</v>
       </c>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I25">
+    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L25">
         <v>0.99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8167AB32-C507-4488-B0C1-5CF207634F21}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,10 +2505,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B3">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2078,10 +2522,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="B4">
-        <v>104</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2095,10 +2539,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="B5">
-        <v>257</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2112,10 +2556,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="B6">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2129,10 +2573,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="B7">
-        <v>976</v>
+        <v>167</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2146,10 +2590,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.99</v>
+        <v>0.8</v>
       </c>
       <c r="B8">
-        <v>1952</v>
+        <v>257</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2158,10 +2602,199 @@
         <v>0.04</v>
       </c>
       <c r="E8">
+        <v>8.3045480000000005E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.85</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.04</v>
+      </c>
+      <c r="E9">
+        <v>8.3045480000000005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>586</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0.04</v>
+      </c>
+      <c r="E10">
+        <v>8.3045480000000005E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.95</v>
+      </c>
+      <c r="B11">
+        <v>976</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0.04</v>
+      </c>
+      <c r="E11">
+        <v>8.3045480000000005E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.99</v>
+      </c>
+      <c r="B12">
+        <v>1952</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0.04</v>
+      </c>
+      <c r="E12">
         <v>8.3045480000000005E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDBD34F-3C17-4DB9-B992-A34A86D32C43}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sim 1 adjust n after adjuster power simulation for k=2
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AC99EF-B6DA-4552-8B14-3CF677200209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BD618-A33C-47F5-AE09-3ED3A9034C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12432" yWindow="1752" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="4" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -667,14 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E3F23-FB2A-4BE0-9E04-457B31D94BA1}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,34 +1136,34 @@
         <v>0.7</v>
       </c>
       <c r="C5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L5">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M5" t="s">
         <v>43</v>
@@ -1185,34 +1177,34 @@
         <v>0.75</v>
       </c>
       <c r="C6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="K6">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L6">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1261,34 +1253,34 @@
         <v>0.85</v>
       </c>
       <c r="C8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="E8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="F8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="G8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="H8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="I8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="J8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="K8">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="L8">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1299,34 +1291,34 @@
         <v>0.9</v>
       </c>
       <c r="C9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="D9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="E9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="F9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="G9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="H9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="I9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="J9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="K9">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="L9">
-        <v>586</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1337,34 +1329,34 @@
         <v>0.95</v>
       </c>
       <c r="C10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="D10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="E10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="F10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="G10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="H10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="I10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="J10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="K10">
-        <v>976</v>
+        <v>925</v>
       </c>
       <c r="L10">
-        <v>976</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1375,34 +1367,34 @@
         <v>0.99</v>
       </c>
       <c r="C11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="D11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="E11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="F11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="G11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="H11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="I11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="J11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="K11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="L11">
-        <v>1952</v>
+        <v>1892</v>
       </c>
       <c r="M11" s="19"/>
     </row>
@@ -1423,104 +1415,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB1F2C-87CD-4737-A94B-BDAF0B0063E4}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="35"/>
-    <col min="2" max="2" width="26.44140625" style="35" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="35"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2">
         <v>55</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2">
         <v>55</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2">
         <v>55</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2">
         <v>55</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2">
         <v>55</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2">
         <v>167</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2">
         <v>167</v>
       </c>
-      <c r="J2" s="35">
+      <c r="J2">
         <v>167</v>
       </c>
-      <c r="K2" s="35">
+      <c r="K2">
         <v>167</v>
       </c>
-      <c r="L2" s="35">
+      <c r="L2">
         <v>167</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+      <c r="A3" s="29">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C3">
@@ -1538,146 +1528,126 @@
       <c r="G3">
         <v>27</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3">
         <v>257</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3">
         <v>257</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3">
         <v>257</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3">
         <v>257</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3">
         <v>257</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="M3" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="33">
+      <c r="A4" s="29">
         <v>3</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4">
         <v>391</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4">
         <v>391</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4">
         <v>391</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4">
         <v>391</v>
       </c>
-      <c r="L4" s="35">
+      <c r="L4">
         <v>391</v>
       </c>
-      <c r="M4" s="34" t="s">
+      <c r="M4" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="36"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="33"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="36"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
add Sim1 for Hc=TRUE to access overall BES-power
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BD618-A33C-47F5-AE09-3ED3A9034C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A77E5-938B-432A-8164-1E4B0BA3FA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12432" yWindow="1752" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t>Condition</t>
   </si>
@@ -426,16 +426,19 @@
     </r>
   </si>
   <si>
-    <t>avg(5x0.65, 5x0.75)=0.7</t>
-  </si>
-  <si>
-    <t>avg(5x0.60, 5x0.80)=0.7</t>
-  </si>
-  <si>
-    <t>avg(5x0.55, 5x0.85)=0.7</t>
-  </si>
-  <si>
     <t>mean=median</t>
+  </si>
+  <si>
+    <t>avg(5x0.70, 5x0.80)=0.75</t>
+  </si>
+  <si>
+    <t>avg(5x0.65, 5x0.85)=0.75</t>
+  </si>
+  <si>
+    <t>avg(5x0.55, 5x0.95)=0.75</t>
+  </si>
+  <si>
+    <t>avg(5x0.60, 5x0.90)=0.76</t>
   </si>
 </sst>
 </file>
@@ -959,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E3F23-FB2A-4BE0-9E04-457B31D94BA1}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" activeCellId="1" sqref="C3 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB1F2C-87CD-4737-A94B-BDAF0B0063E4}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1470,40 +1473,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>102</v>
+      </c>
+      <c r="D2">
+        <v>102</v>
+      </c>
+      <c r="E2">
+        <v>102</v>
+      </c>
+      <c r="F2">
+        <v>102</v>
+      </c>
+      <c r="G2">
+        <v>102</v>
+      </c>
+      <c r="H2">
+        <v>257</v>
+      </c>
+      <c r="I2">
+        <v>257</v>
+      </c>
+      <c r="J2">
+        <v>257</v>
+      </c>
+      <c r="K2">
+        <v>257</v>
+      </c>
+      <c r="L2">
+        <v>257</v>
+      </c>
+      <c r="M2" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="C2">
-        <v>55</v>
-      </c>
-      <c r="D2">
-        <v>55</v>
-      </c>
-      <c r="E2">
-        <v>55</v>
-      </c>
-      <c r="F2">
-        <v>55</v>
-      </c>
-      <c r="G2">
-        <v>55</v>
-      </c>
-      <c r="H2">
-        <v>167</v>
-      </c>
-      <c r="I2">
-        <v>167</v>
-      </c>
-      <c r="J2">
-        <v>167</v>
-      </c>
-      <c r="K2">
-        <v>167</v>
-      </c>
-      <c r="L2">
-        <v>167</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1511,40 +1514,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="F3">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G3">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="H3">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="I3">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="J3">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="K3">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="L3">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1552,51 +1555,88 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>577</v>
+      </c>
+      <c r="I4">
+        <v>577</v>
+      </c>
+      <c r="J4">
+        <v>577</v>
+      </c>
+      <c r="K4">
+        <v>577</v>
+      </c>
+      <c r="L4">
+        <v>577</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="29">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="H4">
-        <v>391</v>
-      </c>
-      <c r="I4">
-        <v>391</v>
-      </c>
-      <c r="J4">
-        <v>391</v>
-      </c>
-      <c r="K4">
-        <v>391</v>
-      </c>
-      <c r="L4">
-        <v>391</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>925</v>
+      </c>
+      <c r="I5">
+        <v>925</v>
+      </c>
+      <c r="J5">
+        <v>925</v>
+      </c>
+      <c r="K5">
+        <v>925</v>
+      </c>
+      <c r="L5">
+        <v>925</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29"/>
       <c r="B7" s="1"/>
     </row>
@@ -1616,38 +1656,56 @@
       <c r="A11" s="29"/>
       <c r="B11" s="1"/>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+    </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
clean up namings across simulations
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5A77E5-938B-432A-8164-1E4B0BA3FA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D38E5AF-E994-485D-A83A-B6EF998CD797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
   <si>
     <t>Condition</t>
   </si>
@@ -438,7 +438,10 @@
     <t>avg(5x0.55, 5x0.95)=0.75</t>
   </si>
   <si>
-    <t>avg(5x0.60, 5x0.90)=0.76</t>
+    <t>avg(10x0.75)=0.75</t>
+  </si>
+  <si>
+    <t>avg(5x0.60, 5x0.90)=0.75</t>
   </si>
 </sst>
 </file>
@@ -963,7 +966,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" activeCellId="1" sqref="C3 C9"/>
+      <selection activeCell="C6" sqref="C6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1416,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB1F2C-87CD-4737-A94B-BDAF0B0063E4}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,83 +1471,83 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="29">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="D2">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="E2">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="F2">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="G2">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="H2">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="I2">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="J2">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="K2">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="L2">
-        <v>257</v>
+        <v>160</v>
       </c>
       <c r="M2" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="D3">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="E3">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="F3">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="G3">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="H3">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="I3">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="J3">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="K3">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="L3">
-        <v>383</v>
+        <v>257</v>
       </c>
       <c r="M3" s="18" t="s">
         <v>62</v>
@@ -1555,37 +1558,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E4">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="F4">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G4">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="H4">
-        <v>577</v>
+        <v>383</v>
       </c>
       <c r="I4">
-        <v>577</v>
+        <v>383</v>
       </c>
       <c r="J4">
-        <v>577</v>
+        <v>383</v>
       </c>
       <c r="K4">
-        <v>577</v>
+        <v>383</v>
       </c>
       <c r="L4">
-        <v>577</v>
+        <v>383</v>
       </c>
       <c r="M4" s="18" t="s">
         <v>62</v>
@@ -1596,51 +1599,88 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H5">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="I5">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="J5">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="K5">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="L5">
-        <v>925</v>
+        <v>577</v>
       </c>
       <c r="M5" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>925</v>
+      </c>
+      <c r="I6">
+        <v>925</v>
+      </c>
+      <c r="J6">
+        <v>925</v>
+      </c>
+      <c r="K6">
+        <v>925</v>
+      </c>
+      <c r="L6">
+        <v>925</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="29"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
       <c r="B8" s="1"/>
     </row>
@@ -1659,9 +1699,10 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1671,18 +1712,17 @@
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
@@ -1694,6 +1734,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
@@ -1706,6 +1747,9 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
not sure what was changed
</commit_message>
<xml_diff>
--- a/Simulations planning.xlsx
+++ b/Simulations planning.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D38E5AF-E994-485D-A83A-B6EF998CD797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAC0935-A186-43AB-96B9-050A5FB0189C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sim1" sheetId="4" r:id="rId1"/>
-    <sheet name="Sim2" sheetId="7" r:id="rId2"/>
-    <sheet name="Sim1_Ntotal=2000" sheetId="1" r:id="rId3"/>
-    <sheet name="Sim1_Ntotal=1000" sheetId="3" r:id="rId4"/>
-    <sheet name="Degrees of power" sheetId="2" r:id="rId5"/>
-    <sheet name="Power quantification" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
+    <sheet name="Sim1.k2" sheetId="4" r:id="rId1"/>
+    <sheet name="Sim1.k3" sheetId="10" r:id="rId2"/>
+    <sheet name="Sim2" sheetId="7" r:id="rId3"/>
+    <sheet name="Sim3" sheetId="9" r:id="rId4"/>
+    <sheet name="SimIdea1" sheetId="8" r:id="rId5"/>
+    <sheet name="Sim1_Ntotal=2000" sheetId="1" state="hidden" r:id="rId6"/>
+    <sheet name="Sim1_Ntotal=1000" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Degrees of power" sheetId="2" state="hidden" r:id="rId8"/>
+    <sheet name="Power quantification" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="55">
   <si>
     <t>Condition</t>
   </si>
@@ -179,253 +181,6 @@
     <t>0.5/0.55</t>
   </si>
   <si>
-    <t>condition    correct.aggr</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color rgb="FF949494"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;chr&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">               </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color rgb="FF949494"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;dbl&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.1         0.605</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.2         0.734</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.3         0.862</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.4         0.932</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.5         0.972</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.6         0.994</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.7         0.998</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.8         1    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> 9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.9         1    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.10        1   </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.1        0.600</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.2        0.740</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.3        0.933</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.4        0.994</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Condition.5        1   </t>
-    </r>
-  </si>
-  <si>
     <t>mean=median</t>
   </si>
   <si>
@@ -442,13 +197,25 @@
   </si>
   <si>
     <t>avg(5x0.60, 5x0.90)=0.75</t>
+  </si>
+  <si>
+    <t>By how much does a single high-powered study improve the BES-power?</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>2:1</t>
+  </si>
+  <si>
+    <t>3:2:1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,27 +237,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF949494"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFBCBCBC"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,14 +293,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -600,11 +342,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,15 +427,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,14 +724,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E3F23-FB2A-4BE0-9E04-457B31D94BA1}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="46.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -983,34 +742,34 @@
       <c r="B1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -1366,40 +1125,40 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="32">
         <v>0.99</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="19">
         <v>1892</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="19">
         <v>1892</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="19">
         <v>1892</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="19">
         <v>1892</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="19">
         <v>1892</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="19">
         <v>1892</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="19">
         <v>1892</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="19">
         <v>1892</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="19">
         <v>1892</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="19">
         <v>1892</v>
       </c>
       <c r="M11" s="19"/>
@@ -1418,11 +1177,495 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9163E431-418E-4D3F-9284-93665075A969}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>15</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>24</v>
+      </c>
+      <c r="J3">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>36</v>
+      </c>
+      <c r="L4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="C5">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <v>51</v>
+      </c>
+      <c r="F5">
+        <v>51</v>
+      </c>
+      <c r="G5">
+        <v>51</v>
+      </c>
+      <c r="H5">
+        <v>51</v>
+      </c>
+      <c r="I5">
+        <v>51</v>
+      </c>
+      <c r="J5">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="29">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C6">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>72</v>
+      </c>
+      <c r="E6">
+        <v>72</v>
+      </c>
+      <c r="F6">
+        <v>72</v>
+      </c>
+      <c r="G6">
+        <v>72</v>
+      </c>
+      <c r="H6">
+        <v>72</v>
+      </c>
+      <c r="I6">
+        <v>72</v>
+      </c>
+      <c r="J6">
+        <v>72</v>
+      </c>
+      <c r="K6">
+        <v>72</v>
+      </c>
+      <c r="L6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C8">
+        <v>135</v>
+      </c>
+      <c r="D8">
+        <v>135</v>
+      </c>
+      <c r="E8">
+        <v>135</v>
+      </c>
+      <c r="F8">
+        <v>135</v>
+      </c>
+      <c r="G8">
+        <v>135</v>
+      </c>
+      <c r="H8">
+        <v>135</v>
+      </c>
+      <c r="I8">
+        <v>135</v>
+      </c>
+      <c r="J8">
+        <v>135</v>
+      </c>
+      <c r="K8">
+        <v>135</v>
+      </c>
+      <c r="L8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C9">
+        <v>188</v>
+      </c>
+      <c r="D9">
+        <v>188</v>
+      </c>
+      <c r="E9">
+        <v>188</v>
+      </c>
+      <c r="F9">
+        <v>188</v>
+      </c>
+      <c r="G9">
+        <v>188</v>
+      </c>
+      <c r="H9">
+        <v>188</v>
+      </c>
+      <c r="I9">
+        <v>188</v>
+      </c>
+      <c r="J9">
+        <v>188</v>
+      </c>
+      <c r="K9">
+        <v>188</v>
+      </c>
+      <c r="L9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>262</v>
+      </c>
+      <c r="D10">
+        <v>262</v>
+      </c>
+      <c r="E10">
+        <v>262</v>
+      </c>
+      <c r="F10">
+        <v>262</v>
+      </c>
+      <c r="G10">
+        <v>262</v>
+      </c>
+      <c r="H10">
+        <v>262</v>
+      </c>
+      <c r="I10">
+        <v>262</v>
+      </c>
+      <c r="J10">
+        <v>262</v>
+      </c>
+      <c r="K10">
+        <v>262</v>
+      </c>
+      <c r="L10">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="C11">
+        <v>420</v>
+      </c>
+      <c r="D11">
+        <v>420</v>
+      </c>
+      <c r="E11">
+        <v>420</v>
+      </c>
+      <c r="F11">
+        <v>420</v>
+      </c>
+      <c r="G11">
+        <v>420</v>
+      </c>
+      <c r="H11">
+        <v>420</v>
+      </c>
+      <c r="I11">
+        <v>420</v>
+      </c>
+      <c r="J11">
+        <v>420</v>
+      </c>
+      <c r="K11">
+        <v>420</v>
+      </c>
+      <c r="L11">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
+        <v>11</v>
+      </c>
+      <c r="B12" s="32">
+        <v>0.99</v>
+      </c>
+      <c r="C12">
+        <v>862</v>
+      </c>
+      <c r="D12">
+        <v>862</v>
+      </c>
+      <c r="E12">
+        <v>862</v>
+      </c>
+      <c r="F12">
+        <v>862</v>
+      </c>
+      <c r="G12">
+        <v>862</v>
+      </c>
+      <c r="H12">
+        <v>862</v>
+      </c>
+      <c r="I12">
+        <v>862</v>
+      </c>
+      <c r="J12">
+        <v>862</v>
+      </c>
+      <c r="K12">
+        <v>862</v>
+      </c>
+      <c r="L12">
+        <v>862</v>
+      </c>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M13" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB1F2C-87CD-4737-A94B-BDAF0B0063E4}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,43 +1674,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1476,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>160</v>
@@ -1490,7 +1733,7 @@
       <c r="F2">
         <v>160</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="30">
         <v>160</v>
       </c>
       <c r="H2">
@@ -1509,7 +1752,7 @@
         <v>160</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1517,7 +1760,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>102</v>
@@ -1531,7 +1774,7 @@
       <c r="F3">
         <v>102</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="30">
         <v>102</v>
       </c>
       <c r="H3">
@@ -1550,7 +1793,7 @@
         <v>257</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1558,7 +1801,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>55</v>
@@ -1572,7 +1815,7 @@
       <c r="F4">
         <v>55</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="30">
         <v>55</v>
       </c>
       <c r="H4">
@@ -1591,7 +1834,7 @@
         <v>383</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1599,7 +1842,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>27</v>
@@ -1613,7 +1856,7 @@
       <c r="F5">
         <v>27</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="30">
         <v>27</v>
       </c>
       <c r="H5">
@@ -1632,48 +1875,48 @@
         <v>577</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="19">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="19">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="19">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="19">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="33">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="19">
         <v>925</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="19">
         <v>925</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="19">
         <v>925</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="19">
         <v>925</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="19">
         <v>925</v>
       </c>
-      <c r="M6" s="18" t="s">
-        <v>62</v>
+      <c r="M6" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1757,7 +2000,166 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA529D7A-73F2-4FF3-A83D-DCD91E760276}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C519ED-5A47-4962-8BD0-F847E7F6AFAF}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>160</v>
+      </c>
+      <c r="D2">
+        <v>160</v>
+      </c>
+      <c r="E2">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>160</v>
+      </c>
+      <c r="G2">
+        <v>160</v>
+      </c>
+      <c r="H2">
+        <v>160</v>
+      </c>
+      <c r="I2">
+        <v>160</v>
+      </c>
+      <c r="J2">
+        <v>160</v>
+      </c>
+      <c r="K2">
+        <v>160</v>
+      </c>
+      <c r="L2">
+        <v>160</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -2177,7 +2579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9070EDF0-829D-4F07-965D-C082A11BFB0B}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -2596,7 +2998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C1D6A-9ED8-4638-8561-F699B52D61B5}">
   <dimension ref="A1:L25"/>
   <sheetViews>
@@ -2818,342 +3220,477 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8167AB32-C507-4488-B0C1-5CF207634F21}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0.5</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0.04</v>
-      </c>
-      <c r="E2">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>0.04</v>
-      </c>
-      <c r="E3">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.6</v>
-      </c>
-      <c r="B4">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.04</v>
-      </c>
-      <c r="E4">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0.65</v>
-      </c>
-      <c r="B5">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0.04</v>
-      </c>
-      <c r="E5">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0.7</v>
-      </c>
-      <c r="B6">
-        <v>104</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0.04</v>
-      </c>
-      <c r="E6">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0.75</v>
-      </c>
-      <c r="B7">
-        <v>167</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0.04</v>
-      </c>
-      <c r="E7">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0.8</v>
-      </c>
-      <c r="B8">
-        <v>257</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>0.04</v>
-      </c>
-      <c r="E8">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0.85</v>
-      </c>
-      <c r="B9">
-        <v>391</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>0.04</v>
-      </c>
-      <c r="E9">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0.9</v>
-      </c>
-      <c r="B10">
-        <v>586</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>0.04</v>
-      </c>
-      <c r="E10">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0.95</v>
-      </c>
-      <c r="B11">
-        <v>976</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>0.04</v>
-      </c>
-      <c r="E11">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0.99</v>
-      </c>
-      <c r="B12">
-        <v>1952</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>0.04</v>
-      </c>
-      <c r="E12">
-        <v>8.3045480000000005E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDBD34F-3C17-4DB9-B992-A34A86D32C43}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="F13" sqref="F13:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
-        <v>45</v>
+      <c r="A1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
-        <v>46</v>
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D2">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>57</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D4">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E4">
         <v>0.6</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>58</v>
+      <c r="F4">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D5">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E5">
         <v>0.65</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>49</v>
+      <c r="F5">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D6">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E6">
         <v>0.7</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>59</v>
+      <c r="F6">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D7">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E7">
         <v>0.75</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="F7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D8">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.8</v>
+      </c>
+      <c r="F8">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D9">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="F9">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D10">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.9</v>
+      </c>
+      <c r="F10">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D11">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.95</v>
+      </c>
+      <c r="F11">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12">
+        <v>4.0978263289430501E-2</v>
+      </c>
+      <c r="D12">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.99</v>
+      </c>
+      <c r="F12">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>0.13</v>
+      </c>
+      <c r="D13">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>0.13</v>
+      </c>
+      <c r="D14">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>0.13</v>
+      </c>
+      <c r="D15">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.6</v>
+      </c>
+      <c r="F15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16">
+        <v>0.13</v>
+      </c>
+      <c r="D16">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.65</v>
+      </c>
+      <c r="F16">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>0.13</v>
+      </c>
+      <c r="D17">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.7</v>
+      </c>
+      <c r="F17">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>0.13</v>
+      </c>
+      <c r="D18">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.75</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19">
+        <v>0.13</v>
+      </c>
+      <c r="D19">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E19">
         <v>0.8</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="F19">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20">
+        <v>0.13</v>
+      </c>
+      <c r="D20">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="F20">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21">
+        <v>0.13</v>
+      </c>
+      <c r="D21">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E21">
         <v>0.9</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="F21">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="C22">
+        <v>0.13</v>
+      </c>
+      <c r="D22">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E22">
         <v>0.95</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="F22">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23">
+        <v>0.13</v>
+      </c>
+      <c r="D23">
+        <v>8.405485E-2</v>
+      </c>
+      <c r="E23">
         <v>0.99</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>56</v>
+      <c r="F23">
+        <v>862</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>